<commit_message>
Change regulator, add rules for pads and vias, update new component to BOM sheet
</commit_message>
<xml_diff>
--- a/AIRUV2_BOM_SEEED_ALL_PARTS.xlsx
+++ b/AIRUV2_BOM_SEEED_ALL_PARTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trentontaylor/Documents/AirU/AirU_v2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\grad-school\laboratory\airQualityControl\repository\airu-board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F41178DC-3002-F845-89C6-F5F5591B2B5B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B49E8D2-090C-4FF0-8564-6B25FF6B2C9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="440" windowWidth="27580" windowHeight="17560" xr2:uid="{446C8397-6FA5-8C49-8D14-9414FBFDBF08}"/>
+    <workbookView xWindow="-37800" yWindow="7275" windowWidth="20910" windowHeight="11835" xr2:uid="{446C8397-6FA5-8C49-8D14-9414FBFDBF08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Designator</t>
   </si>
@@ -117,9 +117,6 @@
     <t>L2</t>
   </si>
   <si>
-    <t>6.8NH 0402</t>
-  </si>
-  <si>
     <t>4.7K 0603</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
   </si>
   <si>
     <t>ACD5036-A3</t>
-  </si>
-  <si>
-    <t>MAX2659</t>
   </si>
   <si>
     <t>TS-1109</t>
@@ -321,6 +315,21 @@
   </si>
   <si>
     <t>microUSB CONNECTOR</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>RESET BUTTON</t>
+  </si>
+  <si>
+    <t>PAM2305AABADJ</t>
+  </si>
+  <si>
+    <t>Voltage regulator</t>
+  </si>
+  <si>
+    <t>4.7uH TDK;VLS201610HBX-4R7M-1</t>
   </si>
 </sst>
 </file>
@@ -363,12 +372,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -423,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -437,17 +458,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -763,21 +786,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CEB962-936C-C34D-8BF2-4F4906C1E459}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="32.5" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.625" customWidth="1"/>
+    <col min="3" max="3" width="8.375" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -807,7 +830,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2">
         <v>302010076</v>
@@ -835,7 +858,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2">
         <v>302010138</v>
@@ -863,7 +886,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2">
         <v>302010139</v>
@@ -877,7 +900,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" s="2">
         <v>302010103</v>
@@ -891,35 +914,35 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2">
         <v>301010292</v>
@@ -933,7 +956,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6">
         <v>301010096</v>
@@ -942,12 +965,12 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2">
         <v>301010090</v>
@@ -961,7 +984,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="2">
         <v>301010163</v>
@@ -975,7 +998,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="6">
         <v>301010291</v>
@@ -984,12 +1007,12 @@
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B16" s="2">
         <v>301010290</v>
@@ -998,12 +1021,12 @@
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" s="2">
         <v>301010299</v>
@@ -1034,18 +1057,18 @@
         <v>29</v>
       </c>
       <c r="B19" s="2">
-        <v>303010682</v>
+        <v>303010544</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2">
         <v>304090044</v>
@@ -1059,7 +1082,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="2">
         <v>304090042</v>
@@ -1072,30 +1095,30 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="A22" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="10">
         <v>304090043</v>
       </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="10">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="2">
+      <c r="A23" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="10">
         <v>304090045</v>
       </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1114,134 +1137,134 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>46</v>
+      <c r="A25" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="10">
+        <v>1</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>47</v>
+      <c r="C27" s="10">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="10">
+        <v>317050012</v>
+      </c>
+      <c r="C29" s="10">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="B29" s="2">
-        <v>317050012</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30" s="11">
+        <v>81</v>
+      </c>
+      <c r="B30" s="9">
         <v>310030097</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="11">
+        <v>83</v>
+      </c>
+      <c r="B31" s="9">
         <v>310070026</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="2">
-        <v>310060024</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>40</v>
+      <c r="A32" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="11">
+        <v>1</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="2">
         <v>318010020</v>
@@ -1250,12 +1273,12 @@
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B35" s="2">
         <v>305010013</v>
@@ -1264,12 +1287,12 @@
         <v>2</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B36" s="2">
         <v>305030000</v>
@@ -1278,12 +1301,12 @@
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="2">
         <v>305030010</v>
@@ -1292,12 +1315,12 @@
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" s="2">
         <v>320020017</v>
@@ -1306,21 +1329,21 @@
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="11">
+        <v>89</v>
+      </c>
+      <c r="B39" s="9">
         <v>320010005</v>
       </c>
       <c r="C39" s="2">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1338,31 +1361,45 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="2">
+      <c r="A41" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="10">
         <v>320170002</v>
       </c>
-      <c r="C41" s="2">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" s="10">
+        <v>1</v>
+      </c>
+      <c r="D41" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17" thickBot="1">
-      <c r="A42" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="10">
+    <row r="42" spans="1:4">
+      <c r="A42" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="11">
+        <v>311020004</v>
+      </c>
+      <c r="C42" s="11">
+        <v>1</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A43" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="8">
         <v>311020024</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C43" s="8">
         <v>2</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>41</v>
+      <c r="D43" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1371,6 +1408,6 @@
     <hyperlink ref="B10" r:id="rId2" display="https://www.digikey.com/product-detail/en/yageo/RC0603JR-0782RL/311-82GRTR-ND/726834" xr:uid="{F7FF9C52-E929-F24F-B034-054CB0C57725}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>